<commit_message>
Added the "Final Demo" question sheet to the excel file
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f879a4f36e1cad25/Documents/Fall 2021/CS341_SoftwareEngineering/Project-12-12/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/910d8b8c7ab06b00/Documents/GitHub/the-chosen-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="230" documentId="8_{2869724F-F399-F247-8D43-910163D6DA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86856E18-C48E-48D7-A632-626E9797AB4F}"/>
+  <xr:revisionPtr revIDLastSave="352" documentId="8_{2869724F-F399-F247-8D43-910163D6DA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0BEF1C4-6227-49A4-A11E-2CFEDF662CCA}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="4365" windowWidth="20865" windowHeight="11835" xr2:uid="{C4618D14-70AD-6D46-854D-BB7035C48A8B}"/>
+    <workbookView xWindow="-80520" yWindow="-8280" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{C4618D14-70AD-6D46-854D-BB7035C48A8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Section 1" sheetId="1" r:id="rId1"/>
     <sheet name="Section 2" sheetId="3" r:id="rId2"/>
+    <sheet name="Final Demo" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="139">
   <si>
     <t>CS 341</t>
   </si>
@@ -356,6 +357,102 @@
   </si>
   <si>
     <t>Nothing</t>
+  </si>
+  <si>
+    <t>How Long Does a Typical New Year's Resolution Last?</t>
+  </si>
+  <si>
+    <t>1 Month</t>
+  </si>
+  <si>
+    <t>1 Week</t>
+  </si>
+  <si>
+    <t>3 Months</t>
+  </si>
+  <si>
+    <t>1 Year</t>
+  </si>
+  <si>
+    <t>2 Weeks</t>
+  </si>
+  <si>
+    <t>Name a Popular Chirstmas Carol</t>
+  </si>
+  <si>
+    <t>"We Wish You a Merry Christmas"</t>
+  </si>
+  <si>
+    <t>"Jingle Bells"</t>
+  </si>
+  <si>
+    <t>"Frosty the Snowman"</t>
+  </si>
+  <si>
+    <t>"Deck the Halls"</t>
+  </si>
+  <si>
+    <t>"Joy to the World"</t>
+  </si>
+  <si>
+    <t>"Santa Claus Is Comin' to Town"</t>
+  </si>
+  <si>
+    <t>"Holly Jolly Christmas"</t>
+  </si>
+  <si>
+    <t>"Silent Night"</t>
+  </si>
+  <si>
+    <t>Name an Item You'd Need to Dress Up as Santa Clause</t>
+  </si>
+  <si>
+    <t>Santa Hat</t>
+  </si>
+  <si>
+    <t>Beard</t>
+  </si>
+  <si>
+    <t>Big Belly</t>
+  </si>
+  <si>
+    <t>Red Coat</t>
+  </si>
+  <si>
+    <t>Red Pants/Belt</t>
+  </si>
+  <si>
+    <t>Suspenders</t>
+  </si>
+  <si>
+    <t>Black Boots</t>
+  </si>
+  <si>
+    <t>Name One of Santa's Reindeer</t>
+  </si>
+  <si>
+    <t>Rudolph</t>
+  </si>
+  <si>
+    <t>Comet</t>
+  </si>
+  <si>
+    <t>Donnor</t>
+  </si>
+  <si>
+    <t>Blitzen</t>
+  </si>
+  <si>
+    <t>Cupid</t>
+  </si>
+  <si>
+    <t>Prancer</t>
+  </si>
+  <si>
+    <t>Dasher</t>
+  </si>
+  <si>
+    <t>Vixen</t>
   </si>
 </sst>
 </file>
@@ -731,7 +828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463D894B-E6A0-2442-98F4-A96EEF85EAFF}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1477,4 +1574,243 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3803244B-6B9F-41DD-BC5C-89834837E2DA}">
+  <dimension ref="A1:O10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="1">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="1">
+        <v>40</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="1">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="1">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="1">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="1">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="1">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="1">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" s="1">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="1">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="1">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" s="1">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="1">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="1">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L10" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>